<commit_message>
Regression analysis to determine Bend Points
</commit_message>
<xml_diff>
--- a/BendPoint.xlsx
+++ b/BendPoint.xlsx
@@ -98,7 +98,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -112,9 +112,10 @@
     <xf numFmtId="3" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -362,7 +363,7 @@
             <c:numRef>
               <c:f>Sheet1!$B$2:$B$40</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="39"/>
                 <c:pt idx="0">
                   <c:v>180</c:v>
@@ -585,7 +586,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -901,9 +902,9 @@
             <c:numRef>
               <c:f>Sheet1!$C$2:$C$40</c:f>
               <c:numCache>
-                <c:formatCode>#,##0</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="39"/>
-                <c:pt idx="0" formatCode="General">
+                <c:pt idx="0">
                   <c:v>1085</c:v>
                 </c:pt>
                 <c:pt idx="1">
@@ -1124,7 +1125,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2698,10 +2699,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F40"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C2"/>
+      <selection activeCell="B2" sqref="B2:B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2738,10 +2739,10 @@
       <c r="A3" s="1">
         <v>1980</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="5">
         <v>194</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="5">
         <v>1171</v>
       </c>
       <c r="D3" s="3"/>
@@ -2752,10 +2753,10 @@
       <c r="A4" s="1">
         <v>1981</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="5">
         <v>211</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="5">
         <v>1274</v>
       </c>
       <c r="D4" s="3"/>
@@ -2766,10 +2767,10 @@
       <c r="A5" s="1">
         <v>1982</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="5">
         <v>230</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="5">
         <v>1388</v>
       </c>
       <c r="D5" s="3"/>
@@ -2780,10 +2781,10 @@
       <c r="A6" s="1">
         <v>1983</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="5">
         <v>254</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="5">
         <v>1528</v>
       </c>
       <c r="D6" s="3"/>
@@ -2794,10 +2795,10 @@
       <c r="A7" s="1">
         <v>1984</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="5">
         <v>267</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="5">
         <v>1612</v>
       </c>
       <c r="D7" s="3"/>
@@ -2808,10 +2809,10 @@
       <c r="A8" s="1">
         <v>1985</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="5">
         <v>280</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="5">
         <v>1691</v>
       </c>
       <c r="D8" s="3"/>
@@ -2822,10 +2823,10 @@
       <c r="A9" s="1">
         <v>1986</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="5">
         <v>297</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="5">
         <v>1790</v>
       </c>
       <c r="D9" s="3"/>
@@ -2836,10 +2837,10 @@
       <c r="A10" s="1">
         <v>1987</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="5">
         <v>310</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="5">
         <v>1866</v>
       </c>
       <c r="D10" s="3"/>
@@ -2850,10 +2851,10 @@
       <c r="A11" s="1">
         <v>1988</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="5">
         <v>319</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="5">
         <v>1922</v>
       </c>
       <c r="D11" s="3"/>
@@ -2864,10 +2865,10 @@
       <c r="A12" s="1">
         <v>1989</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="5">
         <v>339</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="5">
         <v>2044</v>
       </c>
       <c r="D12" s="3"/>
@@ -2878,10 +2879,10 @@
       <c r="A13" s="1">
         <v>1990</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" s="5">
         <v>356</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C13" s="5">
         <v>2145</v>
       </c>
       <c r="D13" s="3"/>
@@ -2892,10 +2893,10 @@
       <c r="A14" s="1">
         <v>1991</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="5">
         <v>370</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C14" s="5">
         <v>2230</v>
       </c>
       <c r="D14" s="3"/>
@@ -2906,10 +2907,10 @@
       <c r="A15" s="1">
         <v>1992</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15" s="5">
         <v>387</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C15" s="5">
         <v>2333</v>
       </c>
       <c r="D15" s="3"/>
@@ -2920,10 +2921,10 @@
       <c r="A16" s="1">
         <v>1993</v>
       </c>
-      <c r="B16" s="3">
+      <c r="B16" s="5">
         <v>401</v>
       </c>
-      <c r="C16" s="4">
+      <c r="C16" s="5">
         <v>2420</v>
       </c>
       <c r="D16" s="3"/>
@@ -2934,10 +2935,10 @@
       <c r="A17" s="1">
         <v>1994</v>
       </c>
-      <c r="B17" s="3">
+      <c r="B17" s="5">
         <v>422</v>
       </c>
-      <c r="C17" s="4">
+      <c r="C17" s="5">
         <v>2545</v>
       </c>
       <c r="D17" s="3"/>
@@ -2948,10 +2949,10 @@
       <c r="A18" s="1">
         <v>1995</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B18" s="5">
         <v>426</v>
       </c>
-      <c r="C18" s="4">
+      <c r="C18" s="5">
         <v>2567</v>
       </c>
       <c r="D18" s="3"/>
@@ -2962,10 +2963,10 @@
       <c r="A19" s="1">
         <v>1996</v>
       </c>
-      <c r="B19" s="3">
+      <c r="B19" s="5">
         <v>437</v>
       </c>
-      <c r="C19" s="4">
+      <c r="C19" s="5">
         <v>2635</v>
       </c>
       <c r="D19" s="3"/>
@@ -2976,10 +2977,10 @@
       <c r="A20" s="1">
         <v>1997</v>
       </c>
-      <c r="B20" s="3">
+      <c r="B20" s="5">
         <v>455</v>
       </c>
-      <c r="C20" s="4">
+      <c r="C20" s="5">
         <v>2741</v>
       </c>
       <c r="D20" s="3"/>
@@ -2990,10 +2991,10 @@
       <c r="A21" s="1">
         <v>1998</v>
       </c>
-      <c r="B21" s="3">
+      <c r="B21" s="5">
         <v>477</v>
       </c>
-      <c r="C21" s="4">
+      <c r="C21" s="5">
         <v>2875</v>
       </c>
       <c r="D21" s="3"/>
@@ -3004,10 +3005,10 @@
       <c r="A22" s="1">
         <v>1999</v>
       </c>
-      <c r="B22" s="3">
+      <c r="B22" s="5">
         <v>505</v>
       </c>
-      <c r="C22" s="4">
+      <c r="C22" s="5">
         <v>3043</v>
       </c>
       <c r="D22" s="3"/>
@@ -3018,10 +3019,10 @@
       <c r="A23" s="1">
         <v>2000</v>
       </c>
-      <c r="B23" s="3">
+      <c r="B23" s="5">
         <v>531</v>
       </c>
-      <c r="C23" s="4">
+      <c r="C23" s="5">
         <v>3202</v>
       </c>
       <c r="D23" s="3"/>
@@ -3032,10 +3033,10 @@
       <c r="A24" s="1">
         <v>2001</v>
       </c>
-      <c r="B24" s="3">
+      <c r="B24" s="5">
         <v>561</v>
       </c>
-      <c r="C24" s="4">
+      <c r="C24" s="5">
         <v>3381</v>
       </c>
       <c r="D24" s="3"/>
@@ -3046,10 +3047,10 @@
       <c r="A25" s="1">
         <v>2002</v>
       </c>
-      <c r="B25" s="3">
+      <c r="B25" s="5">
         <v>592</v>
       </c>
-      <c r="C25" s="4">
+      <c r="C25" s="5">
         <v>3567</v>
       </c>
       <c r="D25" s="3"/>
@@ -3060,10 +3061,10 @@
       <c r="A26" s="1">
         <v>2003</v>
       </c>
-      <c r="B26" s="3">
+      <c r="B26" s="5">
         <v>606</v>
       </c>
-      <c r="C26" s="4">
+      <c r="C26" s="5">
         <v>3653</v>
       </c>
       <c r="D26" s="3"/>
@@ -3074,10 +3075,10 @@
       <c r="A27" s="1">
         <v>2004</v>
       </c>
-      <c r="B27" s="3">
+      <c r="B27" s="5">
         <v>612</v>
       </c>
-      <c r="C27" s="4">
+      <c r="C27" s="5">
         <v>3689</v>
       </c>
       <c r="D27" s="3"/>
@@ -3088,10 +3089,10 @@
       <c r="A28" s="1">
         <v>2005</v>
       </c>
-      <c r="B28" s="3">
+      <c r="B28" s="5">
         <v>627</v>
       </c>
-      <c r="C28" s="4">
+      <c r="C28" s="5">
         <v>3779</v>
       </c>
       <c r="D28" s="3"/>
@@ -3102,10 +3103,10 @@
       <c r="A29" s="1">
         <v>2006</v>
       </c>
-      <c r="B29" s="3">
+      <c r="B29" s="5">
         <v>656</v>
       </c>
-      <c r="C29" s="4">
+      <c r="C29" s="5">
         <v>3955</v>
       </c>
       <c r="D29" s="3"/>
@@ -3116,10 +3117,10 @@
       <c r="A30" s="1">
         <v>2007</v>
       </c>
-      <c r="B30" s="3">
+      <c r="B30" s="5">
         <v>680</v>
       </c>
-      <c r="C30" s="4">
+      <c r="C30" s="5">
         <v>4100</v>
       </c>
       <c r="D30" s="3"/>
@@ -3130,10 +3131,10 @@
       <c r="A31" s="1">
         <v>2008</v>
       </c>
-      <c r="B31" s="3">
+      <c r="B31" s="5">
         <v>711</v>
       </c>
-      <c r="C31" s="4">
+      <c r="C31" s="5">
         <v>4288</v>
       </c>
       <c r="D31" s="3"/>
@@ -3144,10 +3145,10 @@
       <c r="A32" s="1">
         <v>2009</v>
       </c>
-      <c r="B32" s="3">
+      <c r="B32" s="5">
         <v>744</v>
       </c>
-      <c r="C32" s="4">
+      <c r="C32" s="5">
         <v>4483</v>
       </c>
       <c r="D32" s="3"/>
@@ -3158,10 +3159,10 @@
       <c r="A33" s="1">
         <v>2010</v>
       </c>
-      <c r="B33" s="3">
+      <c r="B33" s="5">
         <v>761</v>
       </c>
-      <c r="C33" s="4">
+      <c r="C33" s="5">
         <v>4586</v>
       </c>
       <c r="D33" s="3"/>
@@ -3172,10 +3173,10 @@
       <c r="A34" s="1">
         <v>2011</v>
       </c>
-      <c r="B34" s="3">
+      <c r="B34" s="5">
         <v>749</v>
       </c>
-      <c r="C34" s="4">
+      <c r="C34" s="5">
         <v>4517</v>
       </c>
       <c r="D34" s="3"/>
@@ -3186,10 +3187,10 @@
       <c r="A35" s="1">
         <v>2012</v>
       </c>
-      <c r="B35" s="3">
+      <c r="B35" s="5">
         <v>767</v>
       </c>
-      <c r="C35" s="4">
+      <c r="C35" s="5">
         <v>4624</v>
       </c>
       <c r="D35" s="3"/>
@@ -3200,10 +3201,10 @@
       <c r="A36" s="1">
         <v>2013</v>
       </c>
-      <c r="B36" s="3">
+      <c r="B36" s="5">
         <v>791</v>
       </c>
-      <c r="C36" s="4">
+      <c r="C36" s="5">
         <v>4768</v>
       </c>
       <c r="D36" s="4"/>
@@ -3214,10 +3215,10 @@
       <c r="A37" s="1">
         <v>2014</v>
       </c>
-      <c r="B37" s="3">
+      <c r="B37" s="5">
         <v>816</v>
       </c>
-      <c r="C37" s="4">
+      <c r="C37" s="5">
         <v>4917</v>
       </c>
       <c r="D37" s="4"/>
@@ -3228,10 +3229,10 @@
       <c r="A38" s="1">
         <v>2015</v>
       </c>
-      <c r="B38" s="3">
+      <c r="B38" s="5">
         <v>826</v>
       </c>
-      <c r="C38" s="4">
+      <c r="C38" s="5">
         <v>4980</v>
       </c>
       <c r="D38" s="4"/>
@@ -3242,10 +3243,10 @@
       <c r="A39" s="1">
         <v>2016</v>
       </c>
-      <c r="B39" s="3">
+      <c r="B39" s="5">
         <v>856</v>
       </c>
-      <c r="C39" s="4">
+      <c r="C39" s="5">
         <v>5157</v>
       </c>
       <c r="D39" s="4"/>
@@ -3256,15 +3257,19 @@
       <c r="A40" s="1">
         <v>2017</v>
       </c>
-      <c r="B40" s="3">
+      <c r="B40" s="5">
         <v>885</v>
       </c>
-      <c r="C40" s="4">
+      <c r="C40" s="5">
         <v>5336</v>
       </c>
       <c r="D40" s="4"/>
       <c r="E40" s="4"/>
       <c r="F40" s="4"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B41" s="6"/>
+      <c r="C41" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>